<commit_message>
Add POR pres def, update PID and EHIC fields
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/ehic-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/ehic-dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t xml:space="preserve">pid_id</t>
   </si>
@@ -46,6 +46,12 @@
     <t xml:space="preserve">issuer_institution_code</t>
   </si>
   <si>
+    <t xml:space="preserve">issuer_institution_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document_number</t>
+  </si>
+  <si>
     <t xml:space="preserve">User</t>
   </si>
   <si>
@@ -62,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE Issuing Authority</t>
   </si>
   <si>
     <t xml:space="preserve">john</t>
@@ -88,7 +97,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -119,6 +128,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -238,7 +253,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,6 +311,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,8 +335,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <fgColor rgb="FFF7F7F7"/>
+          <bgColor rgb="FF272727"/>
         </patternFill>
       </fill>
     </dxf>
@@ -340,9 +359,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:J3"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:L3"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="pid_id"/>
     <tableColumn id="2" name="expiry_date"/>
     <tableColumn id="3" name="family_name"/>
@@ -351,35 +370,37 @@
     <tableColumn id="6" name="ssn"/>
     <tableColumn id="7" name="issuer_country"/>
     <tableColumn id="8" name="issuer_institution_code"/>
-    <tableColumn id="9" name="User"/>
-    <tableColumn id="10" name="Password"/>
+    <tableColumn id="9" name="issuer_institution_name"/>
+    <tableColumn id="10" name="document_number"/>
+    <tableColumn id="11" name="User"/>
+    <tableColumn id="12" name="Password"/>
   </tableColumns>
 </table>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="13.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.16"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,25 +425,31 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>33161</v>
@@ -431,30 +458,36 @@
         <v>12313213213</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="9" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="9" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" s="6" t="n">
         <v>33161</v>
@@ -463,16 +496,22 @@
         <v>52313313216</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="15" t="n">
+        <v>987654321</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>18</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add claims on ehic and update svg
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/ehic-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/ehic-dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregorioskatrakazas/Documents/wallet-ecosystem/wallet-enterprise-configurations/issuer/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE087833-5EBC-2543-8C8B-30614CFED59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E76C8E6-2E0B-554F-A76E-A3DF70A970B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22600" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>pid_id</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>issuing_authority_name</t>
+  </si>
+  <si>
+    <t>authentic_source_id</t>
+  </si>
+  <si>
+    <t>authentic_source_name</t>
+  </si>
+  <si>
+    <t>DE Authentic Source</t>
   </si>
 </sst>
 </file>
@@ -300,9 +309,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L3" totalsRowShown="0">
-  <autoFilter ref="A1:L3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N3" totalsRowShown="0">
+  <autoFilter ref="A1:N3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="pid_id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="date_of_expiry"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="family_name"/>
@@ -313,6 +322,8 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="issuing_authority_id"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="issuing_authority_name"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="document_number"/>
+    <tableColumn id="14" xr3:uid="{601E0F96-35E8-BD48-8F82-360466B498F2}" name="authentic_source_id"/>
+    <tableColumn id="15" xr3:uid="{311EF4AC-6B05-3842-8EC6-1E5401D0DA46}" name="authentic_source_name"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="User"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Password"/>
   </tableColumns>
@@ -637,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,12 +662,12 @@
     <col min="7" max="7" width="20.6640625" customWidth="1"/>
     <col min="8" max="8" width="27.1640625" customWidth="1"/>
     <col min="9" max="9" width="25.83203125" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="10" max="12" width="21.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,14 +698,20 @@
       <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -725,14 +742,20 @@
       <c r="J2" s="8">
         <v>123456789</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="8">
+        <v>112233</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -763,10 +786,16 @@
       <c r="J3" s="14">
         <v>987654321</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="14">
+        <v>112233</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add starting and ending dates
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/ehic-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/ehic-dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregorioskatrakazas/Documents/wallet-ecosystem/wallet-enterprise-configurations/issuer/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E76C8E6-2E0B-554F-A76E-A3DF70A970B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0159D78C-BB49-0C48-8AF3-741844A96E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22600" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>pid_id</t>
   </si>
@@ -93,13 +93,10 @@
     <t>issuing_authority_name</t>
   </si>
   <si>
-    <t>authentic_source_id</t>
-  </si>
-  <si>
-    <t>authentic_source_name</t>
-  </si>
-  <si>
-    <t>DE Authentic Source</t>
+    <t>starting_date</t>
+  </si>
+  <si>
+    <t>ending_date</t>
   </si>
 </sst>
 </file>
@@ -274,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,6 +288,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -322,8 +321,8 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="issuing_authority_id"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="issuing_authority_name"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="document_number"/>
-    <tableColumn id="14" xr3:uid="{601E0F96-35E8-BD48-8F82-360466B498F2}" name="authentic_source_id"/>
-    <tableColumn id="15" xr3:uid="{311EF4AC-6B05-3842-8EC6-1E5401D0DA46}" name="authentic_source_name"/>
+    <tableColumn id="13" xr3:uid="{931038E0-B937-6644-84A3-9B625818FA7C}" name="starting_date"/>
+    <tableColumn id="14" xr3:uid="{3EBC2159-1611-5F4D-9445-60DAC38BCC7C}" name="ending_date"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="User"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Password"/>
   </tableColumns>
@@ -650,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,11 +741,11 @@
       <c r="J2" s="8">
         <v>123456789</v>
       </c>
-      <c r="K2" s="8">
-        <v>112233</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>24</v>
+      <c r="K2" s="16">
+        <v>43863</v>
+      </c>
+      <c r="L2" s="16">
+        <v>45690</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>13</v>
@@ -786,11 +785,11 @@
       <c r="J3" s="14">
         <v>987654321</v>
       </c>
-      <c r="K3" s="14">
-        <v>112233</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>24</v>
+      <c r="K3" s="17">
+        <v>43863</v>
+      </c>
+      <c r="L3" s="17">
+        <v>45690</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
add missing authentic source id and name on ehic dataset
</commit_message>
<xml_diff>
--- a/wallet-enterprise-configurations/issuer/dataset/ehic-dataset.xlsx
+++ b/wallet-enterprise-configurations/issuer/dataset/ehic-dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregorioskatrakazas/Documents/wallet-ecosystem/wallet-enterprise-configurations/issuer/dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregorioskatrakazas/Documents/wallet/master/wallet-ecosystem/wallet-enterprise-configurations/issuer/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0159D78C-BB49-0C48-8AF3-741844A96E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD065AF-4AF5-734F-B6D3-FF7EB9ACC3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22600" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>pid_id</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>ending_date</t>
+  </si>
+  <si>
+    <t>authentic_source_id</t>
+  </si>
+  <si>
+    <t>authentic_source_name</t>
+  </si>
+  <si>
+    <t>DE Authentic Source</t>
   </si>
 </sst>
 </file>
@@ -308,9 +317,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N3" totalsRowShown="0">
-  <autoFilter ref="A1:N3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P3" totalsRowShown="0">
+  <autoFilter ref="A1:P3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="pid_id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="date_of_expiry"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="family_name"/>
@@ -320,6 +329,8 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="issuer_country"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="issuing_authority_id"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="issuing_authority_name"/>
+    <tableColumn id="15" xr3:uid="{9EFC2E55-BE22-0642-8A01-637CE0153F6D}" name="authentic_source_id"/>
+    <tableColumn id="16" xr3:uid="{8987046A-A7F5-B545-B99A-5202638DEFDC}" name="authentic_source_name"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="document_number"/>
     <tableColumn id="13" xr3:uid="{931038E0-B937-6644-84A3-9B625818FA7C}" name="starting_date"/>
     <tableColumn id="14" xr3:uid="{3EBC2159-1611-5F4D-9445-60DAC38BCC7C}" name="ending_date"/>
@@ -647,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,13 +671,13 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" customWidth="1"/>
     <col min="8" max="8" width="27.1640625" customWidth="1"/>
-    <col min="9" max="9" width="25.83203125" customWidth="1"/>
-    <col min="10" max="12" width="21.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" customWidth="1"/>
+    <col min="9" max="11" width="25.83203125" customWidth="1"/>
+    <col min="12" max="14" width="21.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,22 +706,28 @@
         <v>21</v>
       </c>
       <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -739,22 +756,28 @@
         <v>12</v>
       </c>
       <c r="J2" s="8">
+        <v>112233</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="8">
         <v>123456789</v>
       </c>
-      <c r="K2" s="16">
+      <c r="M2" s="16">
         <v>43863</v>
       </c>
-      <c r="L2" s="16">
+      <c r="N2" s="16">
         <v>45690</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -783,18 +806,24 @@
         <v>12</v>
       </c>
       <c r="J3" s="14">
+        <v>112233</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="14">
         <v>987654321</v>
       </c>
-      <c r="K3" s="17">
+      <c r="M3" s="17">
         <v>43863</v>
       </c>
-      <c r="L3" s="17">
+      <c r="N3" s="17">
         <v>45690</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="P3" s="15" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>